<commit_message>
added test for oracle (from openshift)
</commit_message>
<xml_diff>
--- a/timings_jsonblobs.xlsx
+++ b/timings_jsonblobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\temp\jsonblobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF376089-561E-4D05-8C0C-AC1632651A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4681CC1A-A82A-4813-B825-3F259DAAEFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13404" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
   </bookViews>
   <sheets>
     <sheet name="timings" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
-  <si>
-    <t>MongoDB (normal)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>MongoDB (compressed)</t>
-  </si>
-  <si>
-    <t>avg json small (ms)</t>
-  </si>
-  <si>
-    <t>avg json medium (ms)</t>
-  </si>
-  <si>
-    <t>avg json large (ms)</t>
   </si>
   <si>
     <r>
@@ -98,28 +86,46 @@
     </r>
   </si>
   <si>
-    <t>WRITE</t>
-  </si>
-  <si>
-    <t>READ</t>
-  </si>
-  <si>
-    <t>Postgres JSONB (flush + object in hibernate cache)</t>
-  </si>
-  <si>
-    <t>Postgres JSONB (flush + lege hibernate cache)</t>
-  </si>
-  <si>
-    <t>Postgres JSON (flush + object in hibernate cache)</t>
-  </si>
-  <si>
-    <t>Postgres JSON (flush + lege hibernate cache)</t>
-  </si>
-  <si>
     <t>local docker</t>
   </si>
   <si>
     <t>Oracle</t>
+  </si>
+  <si>
+    <t>from openshift</t>
+  </si>
+  <si>
+    <t>Postgres JSONB</t>
+  </si>
+  <si>
+    <t>Postgres JSONB (disabled 2nd level hibernate cache)</t>
+  </si>
+  <si>
+    <t>Postgres JSON (disabled 2nd level hibernate cache)</t>
+  </si>
+  <si>
+    <t>Postgres JSON</t>
+  </si>
+  <si>
+    <t>Oracle  (disabled 2nd level hibernate cache)</t>
+  </si>
+  <si>
+    <t>MongoDB (normal, no compression)</t>
+  </si>
+  <si>
+    <t>WRITE (avg ms)</t>
+  </si>
+  <si>
+    <t>READ (avg ms)</t>
+  </si>
+  <si>
+    <t>Json S</t>
+  </si>
+  <si>
+    <t>Json M</t>
+  </si>
+  <si>
+    <t>Json L</t>
   </si>
 </sst>
 </file>
@@ -203,19 +209,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,235 +538,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCB7F3B-FBCA-493E-9123-7AD2DAC8B42F}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" hidden="1" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>210</v>
+      </c>
+      <c r="D3">
+        <v>336</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5">
+        <v>213</v>
+      </c>
+      <c r="D4" s="5">
+        <v>314</v>
+      </c>
+      <c r="E4" s="5">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" hidden="1">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>447</v>
+      </c>
+      <c r="D6">
+        <v>856</v>
+      </c>
+      <c r="E6">
+        <v>0.49</v>
+      </c>
+      <c r="F6">
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>0.03</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5">
+        <v>468</v>
+      </c>
+      <c r="D7" s="5">
+        <v>843</v>
+      </c>
+      <c r="E7" s="5">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5">
+        <v>290</v>
+      </c>
+      <c r="G7" s="5">
+        <v>525</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>325</v>
+      </c>
+      <c r="D8">
+        <v>597</v>
+      </c>
+      <c r="E8">
+        <v>0.48</v>
+      </c>
+      <c r="F8">
+        <v>0.03</v>
+      </c>
+      <c r="G8">
+        <v>0.02</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>315</v>
+      </c>
+      <c r="D9" s="5">
+        <v>542</v>
+      </c>
+      <c r="E9" s="5">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5">
+        <v>117</v>
+      </c>
+      <c r="G9" s="5">
+        <v>220</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
+        <v>127</v>
+      </c>
+      <c r="D11" s="5">
+        <v>206</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>76</v>
+      </c>
+      <c r="G11" s="5">
+        <v>121</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5">
+        <v>58</v>
+      </c>
+      <c r="D12" s="5">
+        <v>86</v>
+      </c>
+      <c r="E12" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F12" s="5">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5">
+        <v>17</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>44</v>
-      </c>
-      <c r="C3">
-        <v>447</v>
-      </c>
-      <c r="D3">
-        <v>856</v>
-      </c>
-      <c r="E3">
-        <v>0.49</v>
-      </c>
-      <c r="F3">
-        <v>0.02</v>
-      </c>
-      <c r="G3">
-        <v>0.03</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7">
-        <v>41</v>
-      </c>
-      <c r="C4" s="7">
-        <v>468</v>
-      </c>
-      <c r="D4" s="7">
-        <v>843</v>
-      </c>
-      <c r="E4" s="7">
-        <v>30.72</v>
-      </c>
-      <c r="F4" s="7">
-        <v>289.70999999999998</v>
-      </c>
-      <c r="G4" s="7">
-        <v>525.29999999999995</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5">
-        <v>325</v>
-      </c>
-      <c r="D5">
-        <v>597</v>
-      </c>
-      <c r="E5">
-        <v>0.48</v>
-      </c>
-      <c r="F5">
-        <v>0.03</v>
-      </c>
-      <c r="G5">
-        <v>0.02</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7">
-        <v>30</v>
-      </c>
-      <c r="C6" s="7">
-        <v>315</v>
-      </c>
-      <c r="D6" s="7">
-        <v>542</v>
-      </c>
-      <c r="E6" s="7">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7">
-        <v>117</v>
-      </c>
-      <c r="G6" s="7">
-        <v>220</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7">
-        <v>127</v>
-      </c>
-      <c r="D7" s="7">
-        <v>206</v>
-      </c>
-      <c r="E7" s="7">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7">
-        <v>76</v>
-      </c>
-      <c r="G7" s="7">
-        <v>121</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7">
-        <v>58</v>
-      </c>
-      <c r="D8" s="7">
-        <v>86</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7">
-        <v>12</v>
-      </c>
-      <c r="G8" s="7">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pgsql json with lz4 compression column
</commit_message>
<xml_diff>
--- a/timings_jsonblobs.xlsx
+++ b/timings_jsonblobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\temp\jsonblobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4681CC1A-A82A-4813-B825-3F259DAAEFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6DDB47-C45B-4C9E-901E-3E2998697B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="14775" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
   </bookViews>
   <sheets>
     <sheet name="timings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>MongoDB (compressed)</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Json L</t>
+  </si>
+  <si>
+    <t>Postgres JSON (disabled 2nd level hibernate cache, lz4 compression)</t>
   </si>
 </sst>
 </file>
@@ -216,14 +219,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCB7F3B-FBCA-493E-9123-7AD2DAC8B42F}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
@@ -557,16 +560,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="B2" s="2" t="s">
@@ -589,7 +592,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" hidden="1" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3">
@@ -752,79 +755,105 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5">
+        <v>271</v>
+      </c>
+      <c r="D10" s="5">
+        <v>470</v>
+      </c>
+      <c r="E10" s="5">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5">
+        <v>130</v>
+      </c>
+      <c r="G10" s="5">
+        <v>242</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
-        <v>127</v>
-      </c>
-      <c r="D11" s="5">
-        <v>206</v>
-      </c>
-      <c r="E11" s="5">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5">
-        <v>76</v>
-      </c>
-      <c r="G11" s="5">
-        <v>121</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="D12" s="5">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="E12" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F12" s="5">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G12" s="5">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>1</v>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5">
+        <v>86</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5">
+        <v>12</v>
+      </c>
+      <c r="G13" s="5">
+        <v>17</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added pgsql bytea with lz4 compression column
</commit_message>
<xml_diff>
--- a/timings_jsonblobs.xlsx
+++ b/timings_jsonblobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\temp\jsonblobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6DDB47-C45B-4C9E-901E-3E2998697B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67953203-6EF7-444A-9057-3C3F3BCA926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="14775" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>MongoDB (compressed)</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Postgres JSON (disabled 2nd level hibernate cache, lz4 compression)</t>
+  </si>
+  <si>
+    <t>Postgres BYTEA (disabled 2nd level hibernate cache, lz4 compression)</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCB7F3B-FBCA-493E-9123-7AD2DAC8B42F}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -781,79 +784,105 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5">
+        <v>131</v>
+      </c>
+      <c r="D11" s="5">
+        <v>262</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5">
+        <v>67</v>
+      </c>
+      <c r="G11" s="5">
+        <v>126</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
-        <v>127</v>
-      </c>
-      <c r="D12" s="5">
-        <v>206</v>
-      </c>
-      <c r="E12" s="5">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5">
-        <v>76</v>
-      </c>
-      <c r="G12" s="5">
-        <v>121</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="D13" s="5">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="E13" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F13" s="5">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G13" s="5">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>1</v>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5">
+        <v>86</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" s="5">
+        <v>12</v>
+      </c>
+      <c r="G14" s="5">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added pgsql lob with lz4 compression column
</commit_message>
<xml_diff>
--- a/timings_jsonblobs.xlsx
+++ b/timings_jsonblobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\temp\jsonblobs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67953203-6EF7-444A-9057-3C3F3BCA926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F042EC2-8F29-40B6-95F8-8841B39D7B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="14775" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
+    <workbookView xWindow="38895" yWindow="1320" windowWidth="23040" windowHeight="11790" xr2:uid="{E763D9FD-9286-47FA-81D2-3D22A406776B}"/>
   </bookViews>
   <sheets>
     <sheet name="timings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>MongoDB (compressed)</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Postgres BYTEA (disabled 2nd level hibernate cache, lz4 compression)</t>
+  </si>
+  <si>
+    <t>Postgres LOB (disabled 2nd level hibernate cache, lz4 compression)</t>
   </si>
 </sst>
 </file>
@@ -544,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCB7F3B-FBCA-493E-9123-7AD2DAC8B42F}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -681,77 +684,77 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="C7" s="5">
-        <v>468</v>
+        <v>1257</v>
       </c>
       <c r="D7" s="5">
-        <v>843</v>
+        <v>2024</v>
       </c>
       <c r="E7" s="5">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="F7" s="5">
-        <v>290</v>
+        <v>1432</v>
       </c>
       <c r="G7" s="5">
-        <v>525</v>
+        <v>2195</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <v>325</v>
-      </c>
-      <c r="D8">
-        <v>597</v>
-      </c>
-      <c r="E8">
-        <v>0.48</v>
-      </c>
-      <c r="F8">
-        <v>0.03</v>
-      </c>
-      <c r="G8">
-        <v>0.02</v>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5">
+        <v>468</v>
+      </c>
+      <c r="D8" s="5">
+        <v>843</v>
+      </c>
+      <c r="E8" s="5">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5">
+        <v>290</v>
+      </c>
+      <c r="G8" s="5">
+        <v>525</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5">
-        <v>315</v>
-      </c>
-      <c r="D9" s="5">
-        <v>542</v>
-      </c>
-      <c r="E9" s="5">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5">
-        <v>117</v>
-      </c>
-      <c r="G9" s="5">
-        <v>220</v>
+    <row r="9" spans="1:8" hidden="1">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>325</v>
+      </c>
+      <c r="D9">
+        <v>597</v>
+      </c>
+      <c r="E9">
+        <v>0.48</v>
+      </c>
+      <c r="F9">
+        <v>0.03</v>
+      </c>
+      <c r="G9">
+        <v>0.02</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>4</v>
@@ -759,25 +762,25 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5">
-        <v>271</v>
+        <v>315</v>
       </c>
       <c r="D10" s="5">
-        <v>470</v>
+        <v>542</v>
       </c>
       <c r="E10" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="5">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G10" s="5">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>4</v>
@@ -785,104 +788,130 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5">
-        <v>131</v>
+        <v>271</v>
       </c>
       <c r="D11" s="5">
-        <v>262</v>
+        <v>470</v>
       </c>
       <c r="E11" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F11" s="5">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="G11" s="5">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5">
+        <v>131</v>
+      </c>
+      <c r="D12" s="5">
+        <v>262</v>
+      </c>
+      <c r="E12" s="5">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5">
+        <v>67</v>
+      </c>
+      <c r="G12" s="5">
+        <v>126</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>127</v>
-      </c>
-      <c r="D13" s="5">
-        <v>206</v>
-      </c>
-      <c r="E13" s="5">
-        <v>8</v>
-      </c>
-      <c r="F13" s="5">
-        <v>76</v>
-      </c>
-      <c r="G13" s="5">
-        <v>121</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="D14" s="5">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="E14" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F14" s="5">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>1</v>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5">
+        <v>58</v>
+      </c>
+      <c r="D15" s="5">
+        <v>86</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5">
+        <v>12</v>
+      </c>
+      <c r="G15" s="5">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>